<commit_message>
National Assembly 2018 PDF files
</commit_message>
<xml_diff>
--- a/data/old_results/__2013 Final cleaned constituency.xlsx
+++ b/data/old_results/__2013 Final cleaned constituency.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\office\Desktop\DI\Zimbabwe_election\data\old_results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{E0EC5EED-14F2-4D41-B48B-BE318F474068}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{A98D353D-E5A9-4E7F-9661-F28CF6B57A3B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="15" windowWidth="18960" windowHeight="11325" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32105,8 +32105,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E9064F4-0229-4469-999C-BB99828FDF56}">
   <dimension ref="A1:R213"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G52" sqref="G52"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.6640625" defaultRowHeight="20.25" x14ac:dyDescent="0.3"/>

</xml_diff>